<commit_message>
Main Menu & Sound Update
- Added Romanian
- Death Ragdolls
- Main Menu
- Credits
- Loading Screen
- Sound effects for punching, damage, fall damage, player voices and death voice
- Music in the Main Menu, Pause Menu and Credit's scene.
</commit_message>
<xml_diff>
--- a/text/translations.xlsx
+++ b/text/translations.xlsx
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="670">
   <si>
     <t>en</t>
   </si>
@@ -1047,9 +1047,6 @@
     <t>Optionsmenü</t>
   </si>
   <si>
-    <t>Menu des options</t>
-  </si>
-  <si>
     <t>オプションメニュー</t>
   </si>
   <si>
@@ -1059,9 +1056,6 @@
     <t>Pause außer Fokus</t>
   </si>
   <si>
-    <t>Pause sans mise au point</t>
-  </si>
-  <si>
     <t>Осветљеност</t>
   </si>
   <si>
@@ -1215,9 +1209,6 @@
     <t>Langue</t>
   </si>
   <si>
-    <t>Console développeur</t>
-  </si>
-  <si>
     <t>Entwicklerkonsole</t>
   </si>
   <si>
@@ -1485,9 +1476,6 @@
     <t>DU MATIN</t>
   </si>
   <si>
-    <t>DE L'APRÈS-MIDI</t>
-  </si>
-  <si>
     <t>Eau</t>
   </si>
   <si>
@@ -1749,9 +1737,6 @@
     <t>Rejoindre</t>
   </si>
   <si>
-    <t>Joueur seul</t>
-  </si>
-  <si>
     <t>Hôte</t>
   </si>
   <si>
@@ -1797,9 +1782,6 @@
     <t>Кредити</t>
   </si>
   <si>
-    <t>Creditos</t>
-  </si>
-  <si>
     <t>§ui§dead</t>
   </si>
   <si>
@@ -1846,13 +1828,310 @@
   </si>
   <si>
     <t>Reaparecew</t>
+  </si>
+  <si>
+    <t>ro</t>
+  </si>
+  <si>
+    <t>Pressione algo... :)</t>
+  </si>
+  <si>
+    <t>§ct§keybind_text</t>
+  </si>
+  <si>
+    <t>Press any key,,, :)</t>
+  </si>
+  <si>
+    <t>Appuyez une touche... :)</t>
+  </si>
+  <si>
+    <t>任意のキーを押してください... :)</t>
+  </si>
+  <si>
+    <t>Apăsați o tastă... :)</t>
+  </si>
+  <si>
+    <t>Drück auf die taste... :)</t>
+  </si>
+  <si>
+    <t>Претисните било који тастер... :)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modul de afișare </t>
+  </si>
+  <si>
+    <t>Luminozitate</t>
+  </si>
+  <si>
+    <t>Aberație Cromatică</t>
+  </si>
+  <si>
+    <t>Pauză fără focalizare</t>
+  </si>
+  <si>
+    <t>Volum Principal</t>
+  </si>
+  <si>
+    <t>Musică</t>
+  </si>
+  <si>
+    <t>Arată FPS</t>
+  </si>
+  <si>
+    <t>Limbă</t>
+  </si>
+  <si>
+    <t>Geam</t>
+  </si>
+  <si>
+    <t>Zoom</t>
+  </si>
+  <si>
+    <t>Opționi</t>
+  </si>
+  <si>
+    <t>Iesi din joc</t>
+  </si>
+  <si>
+    <t>Meniu de Controle</t>
+  </si>
+  <si>
+    <t>Mișcarea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genuflexiune </t>
+  </si>
+  <si>
+    <t>Pauză</t>
+  </si>
+  <si>
+    <t>Consola de Developăr</t>
+  </si>
+  <si>
+    <t>Aleargă</t>
+  </si>
+  <si>
+    <t>Sari</t>
+  </si>
+  <si>
+    <t>Dreapta</t>
+  </si>
+  <si>
+    <t>Stânga</t>
+  </si>
+  <si>
+    <t>Inapoii</t>
+  </si>
+  <si>
+    <t>Inainte</t>
+  </si>
+  <si>
+    <t>Controle</t>
+  </si>
+  <si>
+    <t>Ecran complet</t>
+  </si>
+  <si>
+    <t>§ui§exit_sure_menu</t>
+  </si>
+  <si>
+    <t>Pretende sair do jogo?</t>
+  </si>
+  <si>
+    <t>You want to leave the game?</t>
+  </si>
+  <si>
+    <t>ゲームを終了しますか？</t>
+  </si>
+  <si>
+    <t>Желите ли да изађете из игре?</t>
+  </si>
+  <si>
+    <t>Willst du das Spiel verlassen?</t>
+  </si>
+  <si>
+    <t>DIMINIAȚA</t>
+  </si>
+  <si>
+    <t>Apă</t>
+  </si>
+  <si>
+    <t>Mâncare</t>
+  </si>
+  <si>
+    <t>Da</t>
+  </si>
+  <si>
+    <t>Nu</t>
+  </si>
+  <si>
+    <t>Atacă</t>
+  </si>
+  <si>
+    <t>Perspectivă</t>
+  </si>
+  <si>
+    <t>Puneți adresa aicea</t>
+  </si>
+  <si>
+    <t>Intră</t>
+  </si>
+  <si>
+    <t>Jocați Singuri</t>
+  </si>
+  <si>
+    <t>Gazdă</t>
+  </si>
+  <si>
+    <t>Credite</t>
+  </si>
+  <si>
+    <t>Reapară</t>
+  </si>
+  <si>
+    <t>Viață</t>
+  </si>
+  <si>
+    <t>Piese</t>
+  </si>
+  <si>
+    <t>Ziuă</t>
+  </si>
+  <si>
+    <t>Inainte la Meniu</t>
+  </si>
+  <si>
+    <t>Inapoii la Joc</t>
+  </si>
+  <si>
+    <t>Meniu de Joc</t>
+  </si>
+  <si>
+    <t>Inclinație Laterală de Cameră</t>
+  </si>
+  <si>
+    <t>Viteza Scinbă FOV</t>
+  </si>
+  <si>
+    <t>Arată Viteza</t>
+  </si>
+  <si>
+    <t>Sensibilitate de la Maus</t>
+  </si>
+  <si>
+    <t>Efecte Sonore</t>
+  </si>
+  <si>
+    <t>Meniu de Optioni</t>
+  </si>
+  <si>
+    <t>Rezistență</t>
+  </si>
+  <si>
+    <t>Ați Morit!</t>
+  </si>
+  <si>
+    <t>Sunteti singurii că vreţi să iesiţi din sesie? Progresia voastră nu o să fie salvată!</t>
+  </si>
+  <si>
+    <t>Menu d’Options</t>
+  </si>
+  <si>
+    <t>Pause sans focus</t>
+  </si>
+  <si>
+    <t>Zoomer</t>
+  </si>
+  <si>
+    <t>Console de développeur</t>
+  </si>
+  <si>
+    <t>DU SOIR</t>
+  </si>
+  <si>
+    <t>Jouer Seul</t>
+  </si>
+  <si>
+    <t>intră intr-un Lobby</t>
+  </si>
+  <si>
+    <t>Voulez-vous vraiment quitter?</t>
+  </si>
+  <si>
+    <t>Sunteți sigurii că vreți să iesiți?</t>
+  </si>
+  <si>
+    <t>Moedis</t>
+  </si>
+  <si>
+    <t>Saudi</t>
+  </si>
+  <si>
+    <t>Fulegi</t>
+  </si>
+  <si>
+    <t>Inventari</t>
+  </si>
+  <si>
+    <t>DI TARDI</t>
+  </si>
+  <si>
+    <t>DI MANHAH</t>
+  </si>
+  <si>
+    <t>Agaw</t>
+  </si>
+  <si>
+    <t>Comidi</t>
+  </si>
+  <si>
+    <t>Siah</t>
+  </si>
+  <si>
+    <t>Nadoh</t>
+  </si>
+  <si>
+    <t>Atacaw</t>
+  </si>
+  <si>
+    <t>Perspecitivi</t>
+  </si>
+  <si>
+    <t>Entraw nuah  Lobby</t>
+  </si>
+  <si>
+    <t>Colocaw o enderosogh aqui</t>
+  </si>
+  <si>
+    <t>Entraw</t>
+  </si>
+  <si>
+    <t>Uah Jogadow</t>
+  </si>
+  <si>
+    <t>Anfitiridogh</t>
+  </si>
+  <si>
+    <t>Multijogadow</t>
+  </si>
+  <si>
+    <t>Creditis</t>
+  </si>
+  <si>
+    <t>Pressioni algi... :)</t>
+  </si>
+  <si>
+    <t>Pretendi saiw di jogi?</t>
+  </si>
+  <si>
+    <t>Ti Morresti!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="22">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2013,6 +2292,20 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Liberation Mono;Courier New;Dej"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="33">
@@ -2356,7 +2649,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2372,6 +2665,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2708,10 +3025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D79" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView tabSelected="1" topLeftCell="G37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H89" sqref="H89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="70.7109375" defaultRowHeight="50.1" customHeight="1"/>
@@ -2721,7 +3038,7 @@
     <col min="3" max="16384" width="70.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="50.1" customHeight="1">
+    <row r="1" spans="1:9" ht="50.1" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2741,10 +3058,13 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="50.1" customHeight="1">
+        <v>340</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="50.1" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>80</v>
       </c>
@@ -2755,22 +3075,25 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>311</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>312</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>310</v>
+      <c r="G2" s="7" t="s">
+        <v>639</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="50.1" customHeight="1">
+        <v>377</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="50.1" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -2789,14 +3112,17 @@
       <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="7" t="s">
         <v>282</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="50.1" customHeight="1">
+        <v>341</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="50.1" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -2815,14 +3141,17 @@
       <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="50.1" customHeight="1">
+        <v>342</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="50.1" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -2841,14 +3170,17 @@
       <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="7" t="s">
         <v>283</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="50.1" customHeight="1">
+        <v>378</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="50.1" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -2867,14 +3199,17 @@
       <c r="F6" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="7" t="s">
         <v>284</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="50.1" customHeight="1">
+        <v>379</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="50.1" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -2893,14 +3228,17 @@
       <c r="F7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="50.1" customHeight="1">
+      <c r="I7" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="50.1" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -2919,14 +3257,17 @@
       <c r="F8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="7" t="s">
         <v>23</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="50.1" customHeight="1">
+        <v>380</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="50.1" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -2945,14 +3286,17 @@
       <c r="F9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="7" t="s">
         <v>26</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="50.1" customHeight="1">
+      <c r="I9" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="50.1" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -2966,19 +3310,22 @@
         <v>198</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="7" t="s">
         <v>285</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="50.1" customHeight="1">
+        <v>381</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="50.1" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -2997,14 +3344,17 @@
       <c r="F11" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="7" t="s">
         <v>286</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="50.1" customHeight="1">
+        <v>382</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="50.1" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -3018,19 +3368,22 @@
         <v>200</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>640</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="50.1" customHeight="1">
+        <v>348</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="50.1" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -3049,14 +3402,17 @@
       <c r="F13" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="8" t="s">
         <v>287</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="50.1" customHeight="1">
+        <v>343</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="50.1" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
@@ -3064,25 +3420,28 @@
         <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="7" t="s">
         <v>288</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="50.1" customHeight="1">
+        <v>344</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="50.1" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -3090,25 +3449,28 @@
         <v>42</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>320</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>321</v>
+      <c r="G15" s="7" t="s">
+        <v>319</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="50.1" customHeight="1">
+        <v>383</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="50.1" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
@@ -3119,7 +3481,7 @@
         <v>44</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>44</v>
@@ -3127,14 +3489,17 @@
       <c r="F16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="7" t="s">
         <v>44</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="50.1" customHeight="1">
+      <c r="I16" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="50.1" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -3148,19 +3513,22 @@
         <v>202</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="7" t="s">
         <v>289</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="50.1" customHeight="1">
+        <v>384</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="50.1" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -3174,19 +3542,22 @@
         <v>203</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="7" t="s">
         <v>290</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="50.1" customHeight="1">
+      <c r="I18" s="7" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="50.1" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>51</v>
       </c>
@@ -3205,14 +3576,17 @@
       <c r="F19" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="7" t="s">
         <v>291</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="50.1" customHeight="1">
+        <v>385</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="50.1" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
@@ -3226,19 +3600,22 @@
         <v>205</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>402</v>
+      <c r="G20" s="7" t="s">
+        <v>399</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="50.1" customHeight="1">
+        <v>386</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="50.1" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
@@ -3257,14 +3634,17 @@
       <c r="F21" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="7" t="s">
         <v>292</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="50.1" customHeight="1">
+        <v>387</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="50.1" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>60</v>
       </c>
@@ -3278,45 +3658,51 @@
         <v>207</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="7" t="s">
         <v>293</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="50.1" customHeight="1">
+        <v>388</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="50.1" customHeight="1">
       <c r="A23" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>335</v>
-      </c>
       <c r="D23" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="50.1" customHeight="1">
+      <c r="I23" s="7" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="50.1" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>63</v>
       </c>
@@ -3335,14 +3721,17 @@
       <c r="F24" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="7" t="s">
         <v>294</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="50.1" customHeight="1">
+        <v>345</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="50.1" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
@@ -3361,14 +3750,17 @@
       <c r="F25" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="7" t="s">
         <v>295</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="50.1" customHeight="1">
+        <v>389</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="50.1" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>69</v>
       </c>
@@ -3387,14 +3779,17 @@
       <c r="F26" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" s="7" t="s">
         <v>70</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="50.1" customHeight="1">
+      <c r="I26" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="50.1" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>71</v>
       </c>
@@ -3402,25 +3797,28 @@
         <v>72</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>72</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" s="7" t="s">
         <v>72</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="50.1" customHeight="1">
+        <v>346</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="50.1" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>73</v>
       </c>
@@ -3428,27 +3826,30 @@
         <v>74</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>211</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>74</v>
+      <c r="G28" s="7" t="s">
+        <v>641</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="50.1" customHeight="1">
+        <v>390</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="50.1" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>75</v>
@@ -3465,19 +3866,22 @@
       <c r="F29" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" s="7" t="s">
         <v>296</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="50.1" customHeight="1">
+        <v>349</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="50.1" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>78</v>
@@ -3491,14 +3895,17 @@
       <c r="F30" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="7" t="s">
         <v>297</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="50.1" customHeight="1">
+        <v>350</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="50.1" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>79</v>
       </c>
@@ -3512,19 +3919,22 @@
         <v>214</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" s="7" t="s">
         <v>298</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="50.1" customHeight="1">
+        <v>391</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="50.1" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>86</v>
       </c>
@@ -3543,14 +3953,17 @@
       <c r="F32" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G32" s="7" t="s">
         <v>299</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="50.1" customHeight="1">
+        <v>392</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="50.1" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>87</v>
       </c>
@@ -3569,16 +3982,19 @@
       <c r="F33" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G33" s="7" t="s">
         <v>90</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="50.1" customHeight="1">
+        <v>393</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="50.1" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>88</v>
@@ -3595,19 +4011,22 @@
       <c r="F34" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" s="7" t="s">
         <v>300</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="50.1" customHeight="1">
+        <v>394</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="50.1" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>102</v>
@@ -3621,14 +4040,17 @@
       <c r="F35" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" s="7" t="s">
         <v>301</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="50.1" customHeight="1">
+        <v>395</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="50.1" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>93</v>
       </c>
@@ -3647,14 +4069,17 @@
       <c r="F36" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G36" s="7" t="s">
         <v>302</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="50.1" customHeight="1">
+        <v>396</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="50.1" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>104</v>
       </c>
@@ -3673,14 +4098,17 @@
       <c r="F37" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G37" s="7" t="s">
         <v>303</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="50.1" customHeight="1">
+        <v>351</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="50.1" customHeight="1">
       <c r="A38" s="2" t="s">
         <v>111</v>
       </c>
@@ -3699,14 +4127,17 @@
       <c r="F38" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G38" s="7" t="s">
         <v>304</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="50.1" customHeight="1">
+        <v>352</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="50.1" customHeight="1">
       <c r="A39" s="1" t="s">
         <v>110</v>
       </c>
@@ -3725,14 +4156,17 @@
       <c r="F39" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G39" s="7" t="s">
         <v>305</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="50.1" customHeight="1">
+        <v>353</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="50.1" customHeight="1">
       <c r="A40" s="1" t="s">
         <v>109</v>
       </c>
@@ -3751,14 +4185,17 @@
       <c r="F40" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="G40" s="7" t="s">
         <v>306</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="50.1" customHeight="1">
+        <v>354</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="50.1" customHeight="1">
       <c r="A41" s="1" t="s">
         <v>108</v>
       </c>
@@ -3777,14 +4214,17 @@
       <c r="F41" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G41" s="7" t="s">
         <v>307</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="50.1" customHeight="1">
+        <v>355</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="50.1" customHeight="1">
       <c r="A42" s="1" t="s">
         <v>107</v>
       </c>
@@ -3803,14 +4243,17 @@
       <c r="F42" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G42" s="7" t="s">
         <v>308</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="50.1" customHeight="1">
+        <v>356</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="50.1" customHeight="1">
       <c r="A43" s="1" t="s">
         <v>106</v>
       </c>
@@ -3824,19 +4267,22 @@
         <v>225</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G43" s="7" t="s">
         <v>100</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="50.1" customHeight="1">
+        <v>357</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="50.1" customHeight="1">
       <c r="A44" s="1" t="s">
         <v>105</v>
       </c>
@@ -3855,40 +4301,46 @@
       <c r="F44" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G44" s="7" t="s">
         <v>101</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="50.1" customHeight="1">
+        <v>358</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="50.1" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>338</v>
-      </c>
       <c r="D45" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>642</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="50.1" customHeight="1">
+        <v>347</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="50.1" customHeight="1">
       <c r="A46" s="1" t="s">
         <v>120</v>
       </c>
@@ -3901,11 +4353,12 @@
       <c r="D46" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="G46" s="10"/>
       <c r="H46" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="50.1" customHeight="1">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="50.1" customHeight="1">
       <c r="A47" s="1" t="s">
         <v>136</v>
       </c>
@@ -3918,11 +4371,12 @@
       <c r="D47" s="1" t="s">
         <v>132</v>
       </c>
+      <c r="G47" s="10"/>
       <c r="H47" s="1" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="50.1" customHeight="1">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="50.1" customHeight="1">
       <c r="A48" s="1" t="s">
         <v>137</v>
       </c>
@@ -3935,11 +4389,12 @@
       <c r="D48" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="G48" s="10"/>
       <c r="H48" s="1" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="50.1" customHeight="1">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="50.1" customHeight="1">
       <c r="A49" s="1" t="s">
         <v>138</v>
       </c>
@@ -3952,14 +4407,15 @@
       <c r="D49" s="1" t="s">
         <v>134</v>
       </c>
+      <c r="G49" s="10"/>
       <c r="H49" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="50.1" customHeight="1">
+        <v>366</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="50.1" customHeight="1">
       <c r="A50" s="1" t="s">
         <v>139</v>
       </c>
@@ -3972,11 +4428,12 @@
       <c r="D50" s="1" t="s">
         <v>135</v>
       </c>
+      <c r="G50" s="10"/>
       <c r="H50" s="1" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="50.1" customHeight="1">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="50.1" customHeight="1">
       <c r="A51" s="1" t="s">
         <v>142</v>
       </c>
@@ -3986,11 +4443,12 @@
       <c r="C51" s="1" t="s">
         <v>144</v>
       </c>
+      <c r="G51" s="10"/>
       <c r="H51" s="1" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="50.1" customHeight="1">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="50.1" customHeight="1">
       <c r="A52" s="1" t="s">
         <v>143</v>
       </c>
@@ -4000,11 +4458,12 @@
       <c r="C52" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="G52" s="10"/>
       <c r="H52" s="1" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="50.1" customHeight="1">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="50.1" customHeight="1">
       <c r="A53" s="1" t="s">
         <v>146</v>
       </c>
@@ -4017,11 +4476,13 @@
       <c r="D53" s="1" t="s">
         <v>155</v>
       </c>
+      <c r="G53" s="10"/>
       <c r="H53" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="50.1" customHeight="1">
+        <v>370</v>
+      </c>
+      <c r="I53" s="6"/>
+    </row>
+    <row r="54" spans="1:10" ht="50.1" customHeight="1">
       <c r="A54" s="1" t="s">
         <v>161</v>
       </c>
@@ -4034,11 +4495,12 @@
       <c r="D54" s="1" t="s">
         <v>156</v>
       </c>
+      <c r="G54" s="10"/>
       <c r="H54" s="1" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="50.1" customHeight="1">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="50.1" customHeight="1">
       <c r="A55" s="1" t="s">
         <v>162</v>
       </c>
@@ -4051,11 +4513,12 @@
       <c r="D55" s="1" t="s">
         <v>157</v>
       </c>
+      <c r="G55" s="10"/>
       <c r="H55" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="50.1" customHeight="1">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="50.1" customHeight="1">
       <c r="A56" s="1" t="s">
         <v>163</v>
       </c>
@@ -4068,11 +4531,12 @@
       <c r="D56" s="1" t="s">
         <v>158</v>
       </c>
+      <c r="G56" s="10"/>
       <c r="H56" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="50.1" customHeight="1">
+    <row r="57" spans="1:10" ht="50.1" customHeight="1">
       <c r="A57" s="1" t="s">
         <v>160</v>
       </c>
@@ -4085,11 +4549,12 @@
       <c r="D57" s="1" t="s">
         <v>183</v>
       </c>
+      <c r="G57" s="10"/>
       <c r="H57" s="1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="50.1" customHeight="1">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="50.1" customHeight="1">
       <c r="A58" s="1" t="s">
         <v>170</v>
       </c>
@@ -4102,11 +4567,12 @@
       <c r="D58" s="1" t="s">
         <v>184</v>
       </c>
+      <c r="G58" s="10"/>
       <c r="H58" s="1" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="50.1" customHeight="1">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="50.1" customHeight="1">
       <c r="A59" s="1" t="s">
         <v>171</v>
       </c>
@@ -4119,11 +4585,12 @@
       <c r="D59" s="1" t="s">
         <v>185</v>
       </c>
+      <c r="G59" s="10"/>
       <c r="H59" s="3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="50.1" customHeight="1">
+    <row r="60" spans="1:10" ht="50.1" customHeight="1">
       <c r="A60" s="1" t="s">
         <v>172</v>
       </c>
@@ -4136,11 +4603,12 @@
       <c r="D60" s="1" t="s">
         <v>186</v>
       </c>
+      <c r="G60" s="10"/>
       <c r="H60" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="50.1" customHeight="1">
+    <row r="61" spans="1:10" ht="50.1" customHeight="1">
       <c r="A61" s="1" t="s">
         <v>173</v>
       </c>
@@ -4153,11 +4621,12 @@
       <c r="D61" s="1" t="s">
         <v>187</v>
       </c>
+      <c r="G61" s="10"/>
       <c r="H61" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="50.1" customHeight="1">
+    <row r="62" spans="1:10" ht="50.1" customHeight="1">
       <c r="A62" s="1" t="s">
         <v>174</v>
       </c>
@@ -4170,11 +4639,12 @@
       <c r="D62" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="G62" s="10"/>
       <c r="H62" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="50.1" customHeight="1">
+    <row r="63" spans="1:10" ht="50.1" customHeight="1">
       <c r="A63" s="1" t="s">
         <v>175</v>
       </c>
@@ -4187,633 +4657,764 @@
       <c r="D63" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" ht="50.1" customHeight="1">
+      <c r="G63" s="10"/>
+    </row>
+    <row r="64" spans="1:10" ht="50.1" customHeight="1">
       <c r="A64" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A65" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="G65" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="I65" s="10" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A66" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="G66" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="I66" s="10" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A67" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="I67" s="10" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A68" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>451</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="I68" s="10" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A69" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>432</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>459</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>450</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A65" s="1" t="s">
+      <c r="C69" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="I69" s="10" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A70" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>433</v>
-      </c>
-      <c r="E65" s="4" t="s">
+      <c r="C70" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="G70" s="12" t="s">
+        <v>643</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="I70" s="11" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A71" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="E71" s="4" t="s">
         <v>460</v>
       </c>
-      <c r="F65" s="4" t="s">
-        <v>442</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>451</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A66" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="E66" s="4" t="s">
+      <c r="F71" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="G71" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="I71" s="10" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A72" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="E72" s="4" t="s">
         <v>461</v>
       </c>
-      <c r="F66" s="4" t="s">
-        <v>443</v>
-      </c>
-      <c r="G66" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A67" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>462</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>444</v>
-      </c>
-      <c r="G67" s="4" t="s">
-        <v>453</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A68" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="G68" s="4" t="s">
+      <c r="F72" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="G72" s="12" t="s">
         <v>454</v>
       </c>
-      <c r="H68" s="1" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A69" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>466</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>455</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A70" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>438</v>
-      </c>
-      <c r="E70" s="4" t="s">
+      <c r="H72" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="I72" s="10" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A73" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="F70" s="4" t="s">
-        <v>447</v>
-      </c>
-      <c r="G70" s="4" t="s">
-        <v>456</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A71" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>464</v>
-      </c>
-      <c r="F71" s="4" t="s">
-        <v>448</v>
-      </c>
-      <c r="G71" s="4" t="s">
-        <v>457</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A72" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>440</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>465</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>449</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A73" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="B73" s="4" t="s">
+      <c r="G73" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="I73" s="10" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A74" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="B74" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="G74" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="I74" s="10" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A75" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="G75" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="I75" s="10" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A76" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="D73" s="4" t="s">
-        <v>472</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>473</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="G73" s="4" t="s">
+      <c r="B76" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="G76" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="I76" s="10" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A77" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="G77" s="12" t="s">
+        <v>504</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="I77" s="10" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A78" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>501</v>
+      </c>
+      <c r="G78" s="12" t="s">
+        <v>496</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="I78" s="10" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A79" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="G79" s="12" t="s">
+        <v>537</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="I79" s="13" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A80" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="G80" s="12" t="s">
+        <v>538</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="I80" s="10" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A81" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>527</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="G81" s="12" t="s">
+        <v>539</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="I81" s="10" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A82" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>528</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="G82" s="12" t="s">
+        <v>644</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="I82" s="10" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A83" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>523</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="G83" s="12" t="s">
+        <v>540</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="I83" s="10" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A84" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>530</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="G84" s="12" t="s">
+        <v>541</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="I84" s="10" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A85" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>552</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="G85" s="12" t="s">
+        <v>553</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="I85" s="10" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A86" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="G86" s="12" t="s">
+        <v>565</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="I86" s="10" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A87" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="G87" s="12" t="s">
+        <v>569</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="I87" s="10" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A88" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="H73" s="1" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A74" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="H74" s="1" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A75" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A76" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="H76" s="1" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A77" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>506</v>
-      </c>
-      <c r="E77" s="4" t="s">
-        <v>509</v>
-      </c>
-      <c r="F77" s="4" t="s">
-        <v>504</v>
-      </c>
-      <c r="G77" s="4" t="s">
-        <v>508</v>
-      </c>
-      <c r="H77" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A78" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>507</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>510</v>
-      </c>
-      <c r="F78" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="G78" s="4" t="s">
-        <v>500</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A79" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>522</v>
-      </c>
-      <c r="E79" s="4" t="s">
-        <v>529</v>
-      </c>
-      <c r="F79" s="4" t="s">
-        <v>540</v>
-      </c>
-      <c r="G79" s="4" t="s">
-        <v>541</v>
-      </c>
-      <c r="H79" s="1" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A80" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>524</v>
-      </c>
-      <c r="E80" s="4" t="s">
-        <v>530</v>
-      </c>
-      <c r="F80" s="4" t="s">
-        <v>539</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>542</v>
-      </c>
-      <c r="H80" s="1" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A81" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>525</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>531</v>
-      </c>
-      <c r="F81" s="4" t="s">
-        <v>538</v>
-      </c>
-      <c r="G81" s="4" t="s">
-        <v>543</v>
-      </c>
-      <c r="H81" s="1" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A82" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>526</v>
-      </c>
-      <c r="E82" s="4" t="s">
-        <v>532</v>
-      </c>
-      <c r="F82" s="4" t="s">
-        <v>537</v>
-      </c>
-      <c r="G82" s="4" t="s">
-        <v>544</v>
-      </c>
-      <c r="H82" s="1" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A83" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="D83" s="4" t="s">
-        <v>527</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>533</v>
-      </c>
-      <c r="F83" s="4" t="s">
-        <v>536</v>
-      </c>
-      <c r="G83" s="4" t="s">
-        <v>545</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A84" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>528</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>534</v>
-      </c>
-      <c r="F84" s="4" t="s">
-        <v>535</v>
-      </c>
-      <c r="G84" s="4" t="s">
-        <v>546</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A85" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="D85" s="4" t="s">
-        <v>557</v>
-      </c>
-      <c r="E85" s="4" t="s">
-        <v>559</v>
-      </c>
-      <c r="F85" s="4" t="s">
-        <v>556</v>
-      </c>
-      <c r="G85" s="4" t="s">
-        <v>558</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A86" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>563</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>567</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>573</v>
-      </c>
-      <c r="F86" s="4" t="s">
-        <v>569</v>
-      </c>
-      <c r="G86" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="H86" s="1" t="s">
+      <c r="C88" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A87" s="1" t="s">
-        <v>561</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>564</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="D87" s="4" t="s">
-        <v>568</v>
-      </c>
-      <c r="E87" s="4" t="s">
-        <v>572</v>
-      </c>
-      <c r="F87" s="4" t="s">
-        <v>570</v>
-      </c>
-      <c r="G87" s="4" t="s">
+      <c r="E88" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="G88" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="H87" s="1" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="50.1" customHeight="1">
-      <c r="E88" s="2"/>
+      <c r="H88" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="50.1" customHeight="1">
+      <c r="A89" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="50.1" customHeight="1">
+      <c r="D90" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>